<commit_message>
Relatorio Final - AABA
</commit_message>
<xml_diff>
--- a/Pre_Relatorio_Template.xlsx
+++ b/Pre_Relatorio_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c6096940d94bfb2/Área de Trabalho/ITAU QUANT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_28CC36F9A6024173A48ADBC8253328F82E9286DB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E7D525E-1B7E-4079-A6CC-6E592100EB9F}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_28CC36F9A6024173A48ADBC8253328F82E9286DB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F73421B2-1889-4C68-92C3-DD4B1A92436F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,8 +722,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>

</xml_diff>